<commit_message>
Branch Coverage 누락 수정
Branch Coverage 누락 수정
</commit_message>
<xml_diff>
--- a/ARS_SoftwareUnitTest_Report.xlsx
+++ b/ARS_SoftwareUnitTest_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이종혁\Pictures\Desktop\ARS_Test_Git\SW_Test_Autonomous_Object_Tracking_Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658568E-6741-433C-BD85-67555214A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FCD405-E53E-44A2-882E-09D55FE43569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21495" yWindow="555" windowWidth="21045" windowHeight="14520" activeTab="1" xr2:uid="{9C0766D7-9F8B-4066-86C6-A7E2BEA41E80}"/>
+    <workbookView xWindow="-25410" yWindow="705" windowWidth="21045" windowHeight="14520" activeTab="1" xr2:uid="{9C0766D7-9F8B-4066-86C6-A7E2BEA41E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -357,7 +357,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Project :</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -412,10 +412,6 @@
   </si>
   <si>
     <t>Function</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1465,7 +1461,7 @@
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="C8" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -1610,60 +1606,60 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="F22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="F23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="F25" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="F26" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="F27" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M27" s="5"/>
     </row>
@@ -1706,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADE2C6B-FB98-4B92-AE6C-957801749AFD}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1725,7 +1721,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1733,7 +1729,7 @@
       <c r="E1" s="31"/>
       <c r="F1" s="32"/>
       <c r="G1" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
@@ -1741,7 +1737,7 @@
       <c r="K1" s="31"/>
       <c r="L1" s="32"/>
       <c r="M1" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
@@ -1761,70 +1757,70 @@
         <v>13</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="G2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G3" s="17">
         <v>44906</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I3" s="12">
         <v>5</v>
@@ -1847,35 +1843,35 @@
       <c r="O3" s="14">
         <v>1</v>
       </c>
-      <c r="P3" s="12" t="s">
-        <v>14</v>
+      <c r="P3" s="14">
+        <v>1</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G4" s="17">
         <v>44906</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="9">
         <v>11</v>
@@ -1898,35 +1894,35 @@
       <c r="O4" s="18">
         <v>1</v>
       </c>
-      <c r="P4" s="12" t="s">
-        <v>14</v>
+      <c r="P4" s="14">
+        <v>1</v>
       </c>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G5" s="17">
         <v>44906</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="9">
         <v>14</v>
@@ -1949,35 +1945,35 @@
       <c r="O5" s="18">
         <v>1</v>
       </c>
-      <c r="P5" s="12" t="s">
-        <v>14</v>
+      <c r="P5" s="14">
+        <v>1</v>
       </c>
       <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="D6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G6" s="17">
         <v>44906</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="9">
         <v>8</v>
@@ -2000,35 +1996,35 @@
       <c r="O6" s="18">
         <v>1</v>
       </c>
-      <c r="P6" s="12" t="s">
-        <v>14</v>
+      <c r="P6" s="14">
+        <v>1</v>
       </c>
       <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G7" s="17">
         <v>44910</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="9">
         <v>10</v>
@@ -2051,35 +2047,35 @@
       <c r="O7" s="18">
         <v>1</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>14</v>
+      <c r="P7" s="14">
+        <v>1</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G8" s="17">
         <v>44910</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="9">
         <v>27</v>
@@ -2102,35 +2098,35 @@
       <c r="O8" s="18">
         <v>1</v>
       </c>
-      <c r="P8" s="12" t="s">
-        <v>14</v>
+      <c r="P8" s="14">
+        <v>1</v>
       </c>
       <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G9" s="17">
         <v>44910</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="9">
         <v>15</v>
@@ -2153,35 +2149,35 @@
       <c r="O9" s="18">
         <v>1</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>14</v>
+      <c r="P9" s="14">
+        <v>1</v>
       </c>
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G10" s="17">
         <v>44910</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="9">
         <v>22</v>
@@ -2204,35 +2200,35 @@
       <c r="O10" s="18">
         <v>1</v>
       </c>
-      <c r="P10" s="12" t="s">
-        <v>14</v>
+      <c r="P10" s="14">
+        <v>1</v>
       </c>
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="D11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G11" s="17">
         <v>44910</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="9">
         <v>8</v>
@@ -2255,35 +2251,35 @@
       <c r="O11" s="18">
         <v>1</v>
       </c>
-      <c r="P11" s="12" t="s">
-        <v>14</v>
+      <c r="P11" s="14">
+        <v>1</v>
       </c>
       <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="17">
         <v>44910</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="9">
         <v>13</v>
@@ -2306,8 +2302,8 @@
       <c r="O12" s="18">
         <v>1</v>
       </c>
-      <c r="P12" s="12" t="s">
-        <v>14</v>
+      <c r="P12" s="14">
+        <v>1</v>
       </c>
       <c r="Q12" s="9"/>
     </row>
@@ -2592,7 +2588,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -2608,57 +2604,57 @@
         <v>10</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="16" t="s">
         <v>61</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>